<commit_message>
Update New sensor data
</commit_message>
<xml_diff>
--- a/data/Additional data/13_Cognitive function.xlsx
+++ b/data/Additional data/13_Cognitive function.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24123"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\麻子\Documents\【04】JICA\【08】PBLコース\PBLCourse_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_45BE279242AF000762507F0FDA55A40E8253B52D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cognitive function" sheetId="8" r:id="rId1"/>
@@ -17,10 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cognitive function'!$A$2:$P$14</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -29,27 +39,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
   <si>
+    <t>No</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>被験者ID</t>
+    <rPh sb="0" eb="3">
+      <t>ヒケンシャ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
     <t>確認日
 （ｙｙｙｙ/mm/dd）</t>
     <rPh sb="0" eb="2">
       <t>カクニン</t>
     </rPh>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>被験者ID</t>
-    <rPh sb="0" eb="3">
-      <t>ヒケンシャ</t>
-    </rPh>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>視空間認知機能　11時10分を指す時計を描く（文字盤に数字を全て描く）</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>記憶　読み上げた単語（桜・猫・電車、あるいは、梅・犬・自動車）を覚え、
@@ -60,7 +70,7 @@
     <rPh sb="39" eb="40">
       <t>ヨ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>注意　“７、４、２”と数字を読み上げ、
@@ -68,7 +78,7 @@
     <rPh sb="44" eb="45">
       <t>カイ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>計算　口頭で100から７を引いてもらい
@@ -76,7 +86,7 @@
     <rPh sb="3" eb="5">
       <t>コウトウ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>時計が円形である</t>
@@ -86,15 +96,15 @@
     <rPh sb="4" eb="6">
       <t>エンケイ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>文字盤の数字が過不足無く描かれている</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>長針、短針ともに正しい数字を指している、且つ、短針は長針よりもはっきりと短い、且つ、2 つの針が文字盤の中心でつながっている</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>点数
@@ -111,81 +121,37 @@
     <rPh sb="6" eb="8">
       <t>マンテン</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>結果</t>
     <rPh sb="0" eb="2">
       <t>ケッカ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>点数1</t>
     <rPh sb="0" eb="2">
       <t>テンスウ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>言えなかった言葉に
 ヒントを与えて言えた</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>点数2</t>
     <rPh sb="0" eb="2">
       <t>テンスウ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>cefoxSR1601000702</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707005602</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707005102</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707003502</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707005502</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707004902</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707004502</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707004302</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707005302</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707004802</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707005802</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>cefoxSR1707006002</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <r>
@@ -202,7 +168,7 @@
       </rPr>
       <t>es</t>
     </r>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <r>
@@ -219,76 +185,96 @@
       </rPr>
       <t>o</t>
     </r>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>I can say all three words</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>I was able to do it 3 times</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>I was able to do it 4 times</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707005602</t>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>I can say two words</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>I can say all three words</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707005102</t>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>I can say one word</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>I was able to do it 3 times</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>I was able to do it 2 times</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>I was able to do it 1 time</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707003502</t>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>I was able to do it two or three times</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>I was able to do it 4 times</t>
-    <phoneticPr fontId="7"/>
-  </si>
-  <si>
-    <t>I was able to do it 1 time</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707005502</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707004902</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707004502</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707004302</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707005302</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707005802</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707004802</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>cefoxSR1707006002</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0_ "/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
@@ -442,82 +428,73 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -794,74 +771,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AH21" sqref="AH21"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomLeft" activeCell="AH21" sqref="AH21"/>
       <selection pane="topRight" activeCell="AH21" sqref="AH21"/>
-      <selection pane="bottomLeft" activeCell="AH21" sqref="AH21"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="4.59765625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="32.86328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.46484375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="21.1328125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="5.3984375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="19.3984375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="5.3984375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="41" style="7" customWidth="1"/>
-    <col min="14" max="14" width="10.59765625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="27" style="7" customWidth="1"/>
-    <col min="16" max="16" width="10.59765625" style="7" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="4.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="32.875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="5.375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="19.375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="5.375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="41" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="27" style="6" customWidth="1"/>
+    <col min="16" max="16" width="10.625" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="15" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="15" t="s">
+      <c r="N1" s="14"/>
+      <c r="O1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="17"/>
+      <c r="P1" s="15"/>
     </row>
-    <row r="2" spans="1:16" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="55.5" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -902,563 +878,563 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:16" s="9" customFormat="1">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4">
         <v>44240</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="7">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="10">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7">
         <v>3</v>
       </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11">
+      <c r="K3" s="7"/>
+      <c r="L3" s="8">
         <v>3</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="11">
+        <v>19</v>
+      </c>
+      <c r="N3" s="8">
         <v>3</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="11">
+        <v>20</v>
+      </c>
+      <c r="P3" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
+    <row r="4" spans="1:16">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="4">
         <v>44170</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="10">
-        <v>2</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11">
+        <v>22</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8">
         <v>2</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="11">
+        <v>19</v>
+      </c>
+      <c r="N4" s="8">
         <v>3</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="11">
+        <v>20</v>
+      </c>
+      <c r="P4" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>17</v>
+    <row r="5" spans="1:16" s="9" customFormat="1">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="4">
         <v>44240</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="8">
+        <v>2</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="10">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="10">
-        <v>1</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="11">
-        <v>2</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="4">
         <v>44168</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="23" t="s">
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="7">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8">
+        <v>3</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="8">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="10">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="10">
-        <v>3</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11">
-        <v>3</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="11">
-        <v>3</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="11">
+      <c r="P6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:16">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
+      <c r="B7" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="4">
         <v>44171</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="7">
         <v>2</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="8">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="I7" s="10">
-        <v>3</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11">
-        <v>3</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="11">
-        <v>3</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="C8" s="4">
         <v>44171</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7">
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="10">
+        <v>18</v>
+      </c>
+      <c r="I8" s="7">
         <v>3</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11">
+      <c r="K8" s="7"/>
+      <c r="L8" s="8">
         <v>3</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="11">
+        <v>19</v>
+      </c>
+      <c r="N8" s="8">
         <v>3</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" s="11">
+        <v>20</v>
+      </c>
+      <c r="P8" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:16">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
+      <c r="B9" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="4">
         <v>44171</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7">
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="10">
-        <v>2</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="10">
+        <v>22</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="7">
         <v>1</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="8">
         <v>3</v>
       </c>
       <c r="M9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="8">
+        <v>3</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="N9" s="11">
-        <v>3</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="4">
         <v>44175</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="10">
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="7">
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="10">
+        <v>18</v>
+      </c>
+      <c r="I10" s="7">
         <v>3</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11">
+      <c r="K10" s="7"/>
+      <c r="L10" s="8">
         <v>3</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="11">
+        <v>19</v>
+      </c>
+      <c r="N10" s="8">
         <v>3</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="11">
+        <v>20</v>
+      </c>
+      <c r="P10" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+    <row r="11" spans="1:16">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>23</v>
+      <c r="B11" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="4">
         <v>44175</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10">
+      <c r="D11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7">
         <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="10">
+        <v>18</v>
+      </c>
+      <c r="I11" s="7">
         <v>3</v>
       </c>
       <c r="J11" s="3"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11">
+      <c r="K11" s="7"/>
+      <c r="L11" s="8">
         <v>3</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="11">
+        <v>19</v>
+      </c>
+      <c r="N11" s="8">
         <v>3</v>
       </c>
       <c r="O11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="P11" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="4">
         <v>44202</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="10">
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="7">
         <v>3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="10">
+        <v>18</v>
+      </c>
+      <c r="I12" s="7">
         <v>3</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11">
+      <c r="K12" s="7"/>
+      <c r="L12" s="8">
         <v>3</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="11">
+        <v>19</v>
+      </c>
+      <c r="N12" s="8">
         <v>3</v>
       </c>
       <c r="O12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="P12" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="C13" s="4">
         <v>44171</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="10">
+      <c r="D13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7">
         <v>3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="10">
+        <v>18</v>
+      </c>
+      <c r="I13" s="7">
         <v>3</v>
       </c>
       <c r="J13" s="3"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11">
+      <c r="K13" s="7"/>
+      <c r="L13" s="8">
         <v>3</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="11">
+        <v>19</v>
+      </c>
+      <c r="N13" s="8">
         <v>3</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P13" s="11">
+        <v>20</v>
+      </c>
+      <c r="P13" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+    <row r="14" spans="1:16">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>26</v>
+      <c r="B14" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="C14" s="4">
         <v>44170</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="7">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="8">
+        <v>2</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="10">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="10">
-        <v>2</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11">
-        <v>2</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="11">
-        <v>2</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P14" s="11">
+      <c r="P14" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1472,9 +1448,9 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:L1"/>
   </mergeCells>
-  <phoneticPr fontId="7"/>
+  <phoneticPr fontId="4"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:J12 J8 J3 J6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:J12 J8 J3 J6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"はい,いいえ"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1484,8 +1460,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100AC8664AFD598E6478EDF39439B3209D1" ma:contentTypeVersion="3" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="c5496f946c423db52d300fa4c5cb525f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="864f0d85-d242-45ca-af3f-9d84e3e0da4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ce4e728c247c6006bd6e989f00a2db5" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC8664AFD598E6478EDF39439B3209D1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06c386bccaa1a0dfc607decf1b28aafb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="864f0d85-d242-45ca-af3f-9d84e3e0da4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3be3a601b7e462793c0670d7272fb9ca" ns2:_="">
     <xsd:import namespace="864f0d85-d242-45ca-af3f-9d84e3e0da4d"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1496,6 +1478,7 @@
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1521,6 +1504,11 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -1531,8 +1519,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="コンテンツ タイプ"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="タイトル"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1621,7 +1609,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1630,20 +1618,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2897E1-CC66-40DE-8015-924FCFEAB101}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AF17B28-4141-4050-A0DF-CC2AFE01789B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE3583E8-F29B-472C-B277-AD4081C762FF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90CA1D89-0E88-4E36-918F-EE0C3C64A80A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AF17B28-4141-4050-A0DF-CC2AFE01789B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE3583E8-F29B-472C-B277-AD4081C762FF}"/>
 </file>
</xml_diff>